<commit_message>
bug fixed and removed previous code
</commit_message>
<xml_diff>
--- a/data/input/simulator_scenarios.xlsx
+++ b/data/input/simulator_scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\melodie2\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/CE_RE_AGE/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408B0288-0ED2-4333-B0FA-899666B75718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE81503B-4A97-D04F-8BE3-75E1B01E76F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42320" yWindow="-15680" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulator_scenarios" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -31,22 +31,10 @@
     <t>period_num</t>
   </si>
   <si>
-    <t>period_hours</t>
-  </si>
-  <si>
     <t>agent_num</t>
   </si>
   <si>
-    <t>grid_x_size</t>
-  </si>
-  <si>
-    <t>grid_y_size</t>
-  </si>
-  <si>
-    <t>initial_infected_percentage</t>
-  </si>
-  <si>
-    <t>young_percentage</t>
+    <t>recycle_num</t>
   </si>
   <si>
     <t>network_type</t>
@@ -59,30 +47,6 @@
   </si>
   <si>
     <t>network_param_m</t>
-  </si>
-  <si>
-    <t>vaccination_trust_percentage</t>
-  </si>
-  <si>
-    <t>vaccination_ad_percentage</t>
-  </si>
-  <si>
-    <t>vaccination_ad_success_prob</t>
-  </si>
-  <si>
-    <t>vaccination_neighbor_success_threshold</t>
-  </si>
-  <si>
-    <t>vaccination_action_prob</t>
-  </si>
-  <si>
-    <t>infection_prob</t>
-  </si>
-  <si>
-    <t>reinfection_prob</t>
-  </si>
-  <si>
-    <t>vaccinated_infection_prob</t>
   </si>
   <si>
     <t>barabasi_albert_graph</t>
@@ -99,21 +63,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -139,10 +103,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,29 +379,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="7.125" customWidth="1"/>
-    <col min="4" max="4" width="11.375" customWidth="1"/>
-    <col min="5" max="5" width="9.625" customWidth="1"/>
-    <col min="6" max="7" width="10" customWidth="1"/>
-    <col min="8" max="13" width="23.5" customWidth="1"/>
-    <col min="14" max="16" width="24" customWidth="1"/>
-    <col min="17" max="17" width="32.875" customWidth="1"/>
-    <col min="18" max="18" width="24" customWidth="1"/>
-    <col min="19" max="19" width="18.375" customWidth="1"/>
-    <col min="20" max="20" width="19" customWidth="1"/>
-    <col min="21" max="21" width="21.875" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,10 +414,10 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -465,44 +426,8 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -513,61 +438,25 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
       </c>
       <c r="H2" s="1">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="I2" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1">
-        <v>6</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="M2" s="1">
         <v>2</v>
       </c>
-      <c r="N2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="S2" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -578,62 +467,26 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6</v>
       </c>
       <c r="H3" s="1">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="I3" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="1">
         <v>6</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="M3" s="1">
-        <v>6</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>